<commit_message>
beneficiaries describe themselves on click in listbox
</commit_message>
<xml_diff>
--- a/parameters/beneficiaries.xlsx
+++ b/parameters/beneficiaries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KThom02\fegs-dashboard\parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kthom02\fegs-dashboard\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1094,10 +1094,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1274,10 +1277,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
       </c>
       <c r="C19" t="s">
         <v>36</v>

</xml_diff>